<commit_message>
updates to svf assumptions for parking
</commit_message>
<xml_diff>
--- a/figures/parking-space-SVF.xlsx
+++ b/figures/parking-space-SVF.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cghoehne\GitHub Projects\transport-uhi-phx\figures\"/>
@@ -12,28 +12,32 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13590"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="new" sheetId="2" r:id="rId1"/>
+    <sheet name="old" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="3">
   <si>
     <t>spaces</t>
   </si>
   <si>
-    <t>min</t>
+    <t>min-svf</t>
   </si>
   <si>
-    <t>max</t>
+    <t>max-svf</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -63,9 +67,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -84,6 +89,585 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:srgbClr val="0070C0"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="power"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.22909103273851072"/>
+                  <c:y val="-6.8152596781134972E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="#,##0.0000" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="1200" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="Century Gothic" panose="020B0502020202020204" pitchFamily="34" charset="0"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>new!$A$2:$A$5</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0" formatCode="General">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>100000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>new!$B$2:$B$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0" formatCode="0.0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.15</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-53C7-436A-855F-8F5CD2E59FBA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:srgbClr val="C00000"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="power"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-1.0069225024071553E-3"/>
+                  <c:y val="-0.19365858475763417"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="#,##0.0000" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="Century Gothic" panose="020B0502020202020204" pitchFamily="34" charset="0"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>new!$A$2:$A$5</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0" formatCode="General">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>100000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>new!$C$2:$C$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0" formatCode="0.0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-53C7-436A-855F-8F5CD2E59FBA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="435066536"/>
+        <c:axId val="435066208"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="435066536"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+          <c:max val="100000"/>
+          <c:min val="100"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="Century Gothic" panose="020B0502020202020204" pitchFamily="34" charset="0"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1200"/>
+                  <a:t>Parking</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1200" baseline="0"/>
+                  <a:t> Spaces at Propety</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US" sz="1200"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.29106768763996244"/>
+              <c:y val="0.92455784165318367"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="Century Gothic" panose="020B0502020202020204" pitchFamily="34" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="#,##0" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Century Gothic" panose="020B0502020202020204" pitchFamily="34" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="435066208"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="435066208"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="Century Gothic" panose="020B0502020202020204" pitchFamily="34" charset="0"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1400"/>
+                  <a:t>Parking</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1400" baseline="0"/>
+                  <a:t> Space Sky View Factor (SVF)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US" sz="1400"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="1.2215490514933702E-2"/>
+              <c:y val="6.7958016500310275E-2"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="Century Gothic" panose="020B0502020202020204" pitchFamily="34" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Century Gothic" panose="020B0502020202020204" pitchFamily="34" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="435066536"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr>
+          <a:latin typeface="Century Gothic" panose="020B0502020202020204" pitchFamily="34" charset="0"/>
+        </a:defRPr>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -226,7 +810,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$4</c:f>
+              <c:f>old!$A$2:$A$4</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="3"/>
@@ -244,7 +828,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$2:$C$4</c:f>
+              <c:f>old!$B$2:$B$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -263,7 +847,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-93EB-4143-94FC-FA17CB757890}"/>
+              <c16:uniqueId val="{00000000-98FA-4D60-B377-D3DC77315067}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -382,7 +966,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$4</c:f>
+              <c:f>old!$A$2:$A$4</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="3"/>
@@ -400,7 +984,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$4</c:f>
+              <c:f>old!$C$2:$C$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -419,7 +1003,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-93EB-4143-94FC-FA17CB757890}"/>
+              <c16:uniqueId val="{00000001-98FA-4D60-B377-D3DC77315067}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -785,7 +1369,563 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -1318,7 +2458,44 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>485775</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>180974</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>371475</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>91109</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -1601,10 +2778,71 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet2"/>
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>100</v>
+      </c>
+      <c r="B2" s="2">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>100000</v>
+      </c>
+      <c r="B5">
+        <v>0.15</v>
+      </c>
+      <c r="C5">
+        <v>0.5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1636,10 +2874,10 @@
         <v>10000</v>
       </c>
       <c r="B3">
-        <v>0.75</v>
+        <v>0.5</v>
       </c>
       <c r="C3">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -1647,10 +2885,10 @@
         <v>100000</v>
       </c>
       <c r="B4">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="C4">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
create script to output data tables for appendex, small fixes to SVF parking figure
</commit_message>
<xml_diff>
--- a/figures/parking-space-SVF.xlsx
+++ b/figures/parking-space-SVF.xlsx
@@ -166,12 +166,9 @@
                 <a:lstStyle/>
                 <a:p>
                   <a:pPr>
-                    <a:defRPr sz="1200" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                       <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="65000"/>
-                          <a:lumOff val="35000"/>
-                        </a:schemeClr>
+                        <a:srgbClr val="0070C0"/>
                       </a:solidFill>
                       <a:latin typeface="Century Gothic" panose="020B0502020202020204" pitchFamily="34" charset="0"/>
                       <a:ea typeface="+mn-ea"/>
@@ -267,8 +264,8 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-1.0069225024071553E-3"/>
-                  <c:y val="-0.19365858475763417"/>
+                  <c:x val="-2.0485960408840542E-2"/>
+                  <c:y val="-0.18397126649086165"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="#,##0.0000" sourceLinked="0"/>
@@ -286,10 +283,7 @@
                   <a:pPr>
                     <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                       <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="65000"/>
-                          <a:lumOff val="35000"/>
-                        </a:schemeClr>
+                        <a:srgbClr val="FF0000"/>
                       </a:solidFill>
                       <a:latin typeface="Century Gothic" panose="020B0502020202020204" pitchFamily="34" charset="0"/>
                       <a:ea typeface="+mn-ea"/>
@@ -386,7 +380,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -399,14 +393,9 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US" sz="1200"/>
-                  <a:t>Parking</a:t>
+                  <a:rPr lang="en-US" sz="1000"/>
+                  <a:t>Parking Spaces at Propety</a:t>
                 </a:r>
-                <a:r>
-                  <a:rPr lang="en-US" sz="1200" baseline="0"/>
-                  <a:t> Spaces at Propety</a:t>
-                </a:r>
-                <a:endParaRPr lang="en-US" sz="1200"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -431,7 +420,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
@@ -469,7 +458,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -518,7 +507,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -531,14 +520,9 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US" sz="1400"/>
-                  <a:t>Parking</a:t>
+                  <a:rPr lang="en-US" sz="1000"/>
+                  <a:t>Parking Space Sky View Factor (SVF)</a:t>
                 </a:r>
-                <a:r>
-                  <a:rPr lang="en-US" sz="1400" baseline="0"/>
-                  <a:t> Space Sky View Factor (SVF)</a:t>
-                </a:r>
-                <a:endParaRPr lang="en-US" sz="1400"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -546,8 +530,8 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="1.2215490514933702E-2"/>
-              <c:y val="6.7958016500310275E-2"/>
+              <c:x val="9.1497165335551571E-3"/>
+              <c:y val="0.21659979493481682"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
@@ -563,7 +547,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
@@ -601,7 +585,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -652,7 +636,7 @@
     <a:lstStyle/>
     <a:p>
       <a:pPr>
-        <a:defRPr>
+        <a:defRPr sz="900">
           <a:latin typeface="Century Gothic" panose="020B0502020202020204" pitchFamily="34" charset="0"/>
         </a:defRPr>
       </a:pPr>
@@ -2446,15 +2430,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>485775</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>180974</xdr:rowOff>
+      <xdr:colOff>493102</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>56417</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>371475</xdr:colOff>
+      <xdr:colOff>378802</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>91109</xdr:rowOff>
+      <xdr:rowOff>157052</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2781,8 +2765,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:C2"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>